<commit_message>
fixing error: memperbaiki error di data table student, memperbaiki export dan import data student
</commit_message>
<xml_diff>
--- a/public/assets/excel/Student_Example.xlsx
+++ b/public/assets/excel/Student_Example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Nama</t>
   </si>
@@ -25,6 +25,30 @@
     <t>Password</t>
   </si>
   <si>
+    <t>ClassRoom</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>NIS</t>
+  </si>
+  <si>
+    <t>NISN</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>BirthPlace</t>
+  </si>
+  <si>
+    <t>BirthDate</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
     <t>Bill Cipher</t>
   </si>
   <si>
@@ -37,6 +61,18 @@
     <t>billcipher90</t>
   </si>
   <si>
+    <t>9bb3b722-706d-4d35-bb92-c725b1075357</t>
+  </si>
+  <si>
+    <t>pria</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>Bandung Jawa Barat</t>
+  </si>
+  <si>
     <t>Amorhpous Shape</t>
   </si>
   <si>
@@ -49,6 +85,15 @@
     <t>amorhpusshape90</t>
   </si>
   <si>
+    <t>9bb3b73d-79aa-4d4f-8d6d-adbe487f48f2</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Jakarta Jawa Barat</t>
+  </si>
+  <si>
     <t>Zanthar</t>
   </si>
   <si>
@@ -59,12 +104,27 @@
   </si>
   <si>
     <t>zanthar90</t>
+  </si>
+  <si>
+    <t>9bb3b74e-61f9-435a-91ab-0bc58312a929</t>
+  </si>
+  <si>
+    <t>wanita</t>
+  </si>
+  <si>
+    <t>Sukabumi</t>
+  </si>
+  <si>
+    <t>Sukabumi Jawa Barat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -91,11 +151,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -313,7 +379,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.38"/>
-    <col customWidth="1" min="2" max="5" width="12.63"/>
+    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -329,47 +395,143 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.02110469E8</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4.6491333E7</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8.5727721692E10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3">
+        <v>38353.0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.02110468E8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4.6491334E7</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8.5727721693E10</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3">
+        <v>38354.0</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2.02110467E8</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4.6491335E7</v>
+      </c>
+      <c r="I4" s="1">
+        <v>8.5727721694E10</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="3">
+        <v>38355.0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>

</xml_diff>